<commit_message>
update piti fajar (lunas)
</commit_message>
<xml_diff>
--- a/KAS ASRAMA.xlsx
+++ b/KAS ASRAMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KUMPULAN TUGAS\folder_penting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9749F232-5DBC-418F-8F6F-C071600A28CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42238A16-40E4-4312-B46F-E2ABF9595FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0F8854E5-F826-4F3F-81D4-69C8F4B67C00}"/>
   </bookViews>
@@ -992,16 +992,51 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1013,11 +1048,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1032,45 +1066,11 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1387,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CEDB44F-1E93-417A-80BB-1F4A9B2FB310}">
   <dimension ref="B1:AT55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1449,60 +1449,60 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="73"/>
-      <c r="H3" s="71" t="s">
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="96"/>
+      <c r="H3" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="73"/>
-      <c r="M3" s="71" t="s">
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="96"/>
+      <c r="M3" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="73"/>
-      <c r="R3" s="71" t="s">
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="96"/>
+      <c r="R3" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="72"/>
-      <c r="T3" s="72"/>
-      <c r="U3" s="73"/>
-      <c r="W3" s="71" t="s">
+      <c r="S3" s="95"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="96"/>
+      <c r="W3" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="72"/>
-      <c r="Y3" s="72"/>
-      <c r="Z3" s="73"/>
-      <c r="AB3" s="71" t="s">
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
+      <c r="Z3" s="96"/>
+      <c r="AB3" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="AC3" s="72"/>
-      <c r="AD3" s="72"/>
-      <c r="AE3" s="73"/>
-      <c r="AG3" s="71" t="s">
+      <c r="AC3" s="95"/>
+      <c r="AD3" s="95"/>
+      <c r="AE3" s="96"/>
+      <c r="AG3" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="72"/>
-      <c r="AI3" s="72"/>
-      <c r="AJ3" s="73"/>
-      <c r="AL3" s="71" t="s">
+      <c r="AH3" s="95"/>
+      <c r="AI3" s="95"/>
+      <c r="AJ3" s="96"/>
+      <c r="AL3" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="AM3" s="72"/>
-      <c r="AN3" s="72"/>
-      <c r="AO3" s="73"/>
-      <c r="AQ3" s="71" t="s">
+      <c r="AM3" s="95"/>
+      <c r="AN3" s="95"/>
+      <c r="AO3" s="96"/>
+      <c r="AQ3" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="AR3" s="72"/>
-      <c r="AS3" s="72"/>
-      <c r="AT3" s="73"/>
+      <c r="AR3" s="95"/>
+      <c r="AS3" s="95"/>
+      <c r="AT3" s="96"/>
     </row>
     <row r="4" spans="2:46" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7"/>
@@ -2436,87 +2436,87 @@
     </row>
     <row r="22" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="68"/>
-      <c r="E22" s="69">
+      <c r="D22" s="70"/>
+      <c r="E22" s="97">
         <f>SUM(F5:F21)</f>
         <v>100000</v>
       </c>
-      <c r="F22" s="70"/>
-      <c r="H22" s="67" t="s">
+      <c r="F22" s="98"/>
+      <c r="H22" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="68"/>
-      <c r="J22" s="69">
+      <c r="I22" s="70"/>
+      <c r="J22" s="97">
         <f>SUM(K5:K21)</f>
         <v>50000</v>
       </c>
-      <c r="K22" s="70"/>
-      <c r="M22" s="67" t="s">
+      <c r="K22" s="98"/>
+      <c r="M22" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="N22" s="68"/>
-      <c r="O22" s="69">
+      <c r="N22" s="70"/>
+      <c r="O22" s="97">
         <f>SUM(P5:P21)</f>
         <v>0</v>
       </c>
-      <c r="P22" s="70"/>
-      <c r="R22" s="67" t="s">
+      <c r="P22" s="98"/>
+      <c r="R22" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="S22" s="68"/>
-      <c r="T22" s="69">
+      <c r="S22" s="70"/>
+      <c r="T22" s="97">
         <f>SUM(U5:U21)</f>
         <v>100000</v>
       </c>
-      <c r="U22" s="70"/>
-      <c r="W22" s="67" t="s">
+      <c r="U22" s="98"/>
+      <c r="W22" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="X22" s="68"/>
-      <c r="Y22" s="69">
+      <c r="X22" s="70"/>
+      <c r="Y22" s="97">
         <f>SUM(Z5:Z21)</f>
         <v>150000</v>
       </c>
-      <c r="Z22" s="70"/>
-      <c r="AB22" s="67" t="s">
+      <c r="Z22" s="98"/>
+      <c r="AB22" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="AC22" s="68"/>
-      <c r="AD22" s="69">
+      <c r="AC22" s="70"/>
+      <c r="AD22" s="97">
         <f>SUM(AE5:AE21)</f>
         <v>150000</v>
       </c>
-      <c r="AE22" s="70"/>
-      <c r="AG22" s="67" t="s">
+      <c r="AE22" s="98"/>
+      <c r="AG22" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="AH22" s="68"/>
-      <c r="AI22" s="69">
+      <c r="AH22" s="70"/>
+      <c r="AI22" s="97">
         <f>SUM(AJ5:AJ21)</f>
         <v>100000</v>
       </c>
-      <c r="AJ22" s="70"/>
-      <c r="AL22" s="67" t="s">
+      <c r="AJ22" s="98"/>
+      <c r="AL22" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="AM22" s="68"/>
-      <c r="AN22" s="69">
+      <c r="AM22" s="70"/>
+      <c r="AN22" s="97">
         <f>SUM(AO5:AO21)</f>
         <v>60000</v>
       </c>
-      <c r="AO22" s="70"/>
-      <c r="AQ22" s="67" t="s">
+      <c r="AO22" s="98"/>
+      <c r="AQ22" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="AR22" s="68"/>
-      <c r="AS22" s="69">
+      <c r="AR22" s="70"/>
+      <c r="AS22" s="97">
         <f>SUM(AT5:AT21)</f>
         <v>150000</v>
       </c>
-      <c r="AT22" s="70"/>
+      <c r="AT22" s="98"/>
     </row>
     <row r="23" spans="2:46" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
@@ -2525,25 +2525,25 @@
       <c r="B24" s="1"/>
     </row>
     <row r="25" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="M25" s="83" t="s">
+      <c r="M25" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="N25" s="84"/>
-      <c r="O25" s="84"/>
-      <c r="P25" s="85"/>
-      <c r="R25" s="83" t="s">
+      <c r="N25" s="90"/>
+      <c r="O25" s="90"/>
+      <c r="P25" s="91"/>
+      <c r="R25" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="S25" s="84"/>
-      <c r="T25" s="84"/>
-      <c r="U25" s="85"/>
+      <c r="S25" s="90"/>
+      <c r="T25" s="90"/>
+      <c r="U25" s="91"/>
     </row>
     <row r="26" spans="2:46" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G26" s="80" t="s">
+      <c r="G26" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="H26" s="81"/>
-      <c r="I26" s="82"/>
+      <c r="H26" s="101"/>
+      <c r="I26" s="102"/>
       <c r="M26" s="36" t="s">
         <v>20</v>
       </c>
@@ -2577,21 +2577,21 @@
       <c r="AA26" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AB26" s="98" t="s">
+      <c r="AB26" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="AC26" s="99"/>
+      <c r="AC26" s="79"/>
       <c r="AH26" s="56"/>
     </row>
     <row r="27" spans="2:46" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="99"/>
       <c r="E27" s="25">
         <f>SUM(E22+J22+O22+T22+Y22+AD22+AI22+AN22+AS22+I45)</f>
-        <v>1095500</v>
+        <v>1106500</v>
       </c>
       <c r="G27" s="26" t="s">
         <v>7</v>
@@ -2605,20 +2605,20 @@
       <c r="M27" s="13">
         <v>1</v>
       </c>
-      <c r="N27" s="76" t="s">
+      <c r="N27" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="O27" s="76"/>
+      <c r="O27" s="103"/>
       <c r="P27" s="14">
         <v>8500</v>
       </c>
       <c r="R27" s="13">
         <v>1</v>
       </c>
-      <c r="S27" s="75">
+      <c r="S27" s="104">
         <v>45691</v>
       </c>
-      <c r="T27" s="76"/>
+      <c r="T27" s="103"/>
       <c r="U27" s="45">
         <v>5000</v>
       </c>
@@ -2628,17 +2628,17 @@
       <c r="X27" s="13">
         <v>1</v>
       </c>
-      <c r="Y27" s="95">
+      <c r="Y27" s="82">
         <v>45727</v>
       </c>
-      <c r="Z27" s="96"/>
+      <c r="Z27" s="83"/>
       <c r="AA27" s="45">
         <v>5000</v>
       </c>
-      <c r="AB27" s="100" t="s">
+      <c r="AB27" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="AC27" s="101"/>
+      <c r="AC27" s="81"/>
       <c r="AH27" s="56"/>
       <c r="AN27" t="s">
         <v>59</v>
@@ -2657,20 +2657,20 @@
       <c r="M28" s="15">
         <v>2</v>
       </c>
-      <c r="N28" s="74" t="s">
+      <c r="N28" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="O28" s="74"/>
+      <c r="O28" s="85"/>
       <c r="P28" s="16">
         <v>290000</v>
       </c>
       <c r="R28" s="13">
         <v>2</v>
       </c>
-      <c r="S28" s="77">
+      <c r="S28" s="84">
         <v>45692</v>
       </c>
-      <c r="T28" s="74"/>
+      <c r="T28" s="85"/>
       <c r="U28" s="46">
         <v>5000</v>
       </c>
@@ -2680,25 +2680,25 @@
       <c r="X28" s="13">
         <v>2</v>
       </c>
-      <c r="Y28" s="93">
+      <c r="Y28" s="74">
         <v>45729</v>
       </c>
-      <c r="Z28" s="94"/>
+      <c r="Z28" s="75"/>
       <c r="AA28" s="45">
         <v>5000</v>
       </c>
-      <c r="AB28" s="100" t="s">
+      <c r="AB28" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="AC28" s="101"/>
+      <c r="AC28" s="81"/>
       <c r="AH28" s="56"/>
     </row>
     <row r="29" spans="2:46" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="79" t="s">
+      <c r="B29" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="79"/>
-      <c r="D29" s="79"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="99"/>
       <c r="E29" s="25">
         <f>(P55+U55+AA55)</f>
         <v>905500</v>
@@ -2710,25 +2710,25 @@
         <v>30</v>
       </c>
       <c r="I29" s="32">
-        <v>230500</v>
+        <v>241500</v>
       </c>
       <c r="M29" s="31">
         <v>3</v>
       </c>
-      <c r="N29" s="91" t="s">
+      <c r="N29" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="O29" s="92"/>
+      <c r="O29" s="93"/>
       <c r="P29" s="32">
         <v>18000</v>
       </c>
       <c r="R29" s="13">
         <v>3</v>
       </c>
-      <c r="S29" s="77">
+      <c r="S29" s="84">
         <v>45693</v>
       </c>
-      <c r="T29" s="74"/>
+      <c r="T29" s="85"/>
       <c r="U29" s="46">
         <v>5000</v>
       </c>
@@ -2738,17 +2738,17 @@
       <c r="X29" s="13">
         <v>3</v>
       </c>
-      <c r="Y29" s="93">
+      <c r="Y29" s="74">
         <v>45731</v>
       </c>
-      <c r="Z29" s="94"/>
+      <c r="Z29" s="75"/>
       <c r="AA29" s="45">
         <v>5000</v>
       </c>
-      <c r="AB29" s="86" t="s">
+      <c r="AB29" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="AC29" s="97"/>
+      <c r="AC29" s="68"/>
       <c r="AH29" s="56"/>
       <c r="AN29" t="s">
         <v>38</v>
@@ -2764,20 +2764,20 @@
       <c r="M30" s="15">
         <v>4</v>
       </c>
-      <c r="N30" s="74" t="s">
+      <c r="N30" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="O30" s="74"/>
+      <c r="O30" s="85"/>
       <c r="P30" s="16">
         <v>102000</v>
       </c>
       <c r="R30" s="13">
         <v>4</v>
       </c>
-      <c r="S30" s="77">
+      <c r="S30" s="84">
         <v>45694</v>
       </c>
-      <c r="T30" s="74"/>
+      <c r="T30" s="85"/>
       <c r="U30" s="46">
         <v>5000</v>
       </c>
@@ -2787,17 +2787,17 @@
       <c r="X30" s="13">
         <v>4</v>
       </c>
-      <c r="Y30" s="93">
+      <c r="Y30" s="74">
         <v>45733</v>
       </c>
-      <c r="Z30" s="94"/>
+      <c r="Z30" s="75"/>
       <c r="AA30" s="45">
         <v>5000</v>
       </c>
-      <c r="AB30" s="86" t="s">
+      <c r="AB30" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="AC30" s="97"/>
+      <c r="AC30" s="68"/>
       <c r="AH30" s="56"/>
       <c r="AN30" t="s">
         <v>60</v>
@@ -2807,14 +2807,14 @@
       </c>
     </row>
     <row r="31" spans="2:46" x14ac:dyDescent="0.35">
-      <c r="B31" s="78" t="s">
+      <c r="B31" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
+      <c r="C31" s="105"/>
+      <c r="D31" s="105"/>
       <c r="E31" s="24">
         <f>(E27-E29)</f>
-        <v>190000</v>
+        <v>201000</v>
       </c>
       <c r="G31" s="31"/>
       <c r="H31" s="28"/>
@@ -2822,20 +2822,20 @@
       <c r="M31" s="15">
         <v>5</v>
       </c>
-      <c r="N31" s="74" t="s">
+      <c r="N31" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="O31" s="74"/>
+      <c r="O31" s="85"/>
       <c r="P31" s="16">
         <v>3000</v>
       </c>
       <c r="R31" s="13">
         <v>5</v>
       </c>
-      <c r="S31" s="77">
+      <c r="S31" s="84">
         <v>45695</v>
       </c>
-      <c r="T31" s="74"/>
+      <c r="T31" s="85"/>
       <c r="U31" s="46">
         <v>5000</v>
       </c>
@@ -2845,17 +2845,17 @@
       <c r="X31" s="13">
         <v>5</v>
       </c>
-      <c r="Y31" s="93">
+      <c r="Y31" s="74">
         <v>45736</v>
       </c>
-      <c r="Z31" s="94"/>
+      <c r="Z31" s="75"/>
       <c r="AA31" s="45">
         <v>5000</v>
       </c>
-      <c r="AB31" s="86" t="s">
+      <c r="AB31" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="AC31" s="97"/>
+      <c r="AC31" s="68"/>
       <c r="AH31" s="56"/>
       <c r="AN31" t="s">
         <v>40</v>
@@ -2871,20 +2871,20 @@
       <c r="M32" s="15">
         <v>6</v>
       </c>
-      <c r="N32" s="74" t="s">
+      <c r="N32" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="O32" s="74"/>
+      <c r="O32" s="85"/>
       <c r="P32" s="16">
         <v>10000</v>
       </c>
       <c r="R32" s="13">
         <v>6</v>
       </c>
-      <c r="S32" s="77">
+      <c r="S32" s="84">
         <v>45696</v>
       </c>
-      <c r="T32" s="74"/>
+      <c r="T32" s="85"/>
       <c r="U32" s="46">
         <v>5000</v>
       </c>
@@ -2894,17 +2894,17 @@
       <c r="X32" s="13">
         <v>6</v>
       </c>
-      <c r="Y32" s="93">
+      <c r="Y32" s="74">
         <v>45741</v>
       </c>
-      <c r="Z32" s="94"/>
+      <c r="Z32" s="75"/>
       <c r="AA32" s="45">
         <v>5000</v>
       </c>
-      <c r="AB32" s="86" t="s">
+      <c r="AB32" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="AC32" s="97"/>
+      <c r="AC32" s="68"/>
       <c r="AH32" s="56"/>
       <c r="AN32" t="s">
         <v>42</v>
@@ -2920,20 +2920,20 @@
       <c r="M33" s="15">
         <v>7</v>
       </c>
-      <c r="N33" s="74" t="s">
+      <c r="N33" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="O33" s="74"/>
+      <c r="O33" s="85"/>
       <c r="P33" s="16">
         <v>102000</v>
       </c>
       <c r="R33" s="13">
         <v>7</v>
       </c>
-      <c r="S33" s="77">
+      <c r="S33" s="84">
         <v>45697</v>
       </c>
-      <c r="T33" s="74"/>
+      <c r="T33" s="85"/>
       <c r="U33" s="46">
         <v>5000</v>
       </c>
@@ -2943,17 +2943,17 @@
       <c r="X33" s="13">
         <v>7</v>
       </c>
-      <c r="Y33" s="93">
+      <c r="Y33" s="74">
         <v>45752</v>
       </c>
-      <c r="Z33" s="94"/>
+      <c r="Z33" s="75"/>
       <c r="AA33" s="45">
         <v>5000</v>
       </c>
-      <c r="AB33" s="86" t="s">
+      <c r="AB33" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="AC33" s="97"/>
+      <c r="AC33" s="68"/>
       <c r="AH33" s="56"/>
       <c r="AN33" t="s">
         <v>36</v>
@@ -2969,20 +2969,20 @@
       <c r="M34" s="15">
         <v>8</v>
       </c>
-      <c r="N34" s="74" t="s">
+      <c r="N34" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="O34" s="74"/>
+      <c r="O34" s="85"/>
       <c r="P34" s="16">
         <v>40000</v>
       </c>
       <c r="R34" s="13">
         <v>8</v>
       </c>
-      <c r="S34" s="77">
+      <c r="S34" s="84">
         <v>45699</v>
       </c>
-      <c r="T34" s="74"/>
+      <c r="T34" s="85"/>
       <c r="U34" s="46">
         <v>5000</v>
       </c>
@@ -2992,17 +2992,17 @@
       <c r="X34" s="13">
         <v>8</v>
       </c>
-      <c r="Y34" s="93">
+      <c r="Y34" s="74">
         <v>45755</v>
       </c>
-      <c r="Z34" s="94"/>
+      <c r="Z34" s="75"/>
       <c r="AA34" s="45">
         <v>5000</v>
       </c>
-      <c r="AB34" s="100" t="s">
+      <c r="AB34" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="AC34" s="101"/>
+      <c r="AC34" s="81"/>
       <c r="AH34" s="56"/>
     </row>
     <row r="35" spans="7:41" x14ac:dyDescent="0.35">
@@ -3021,10 +3021,10 @@
       <c r="R35" s="13">
         <v>9</v>
       </c>
-      <c r="S35" s="77">
+      <c r="S35" s="84">
         <v>45700</v>
       </c>
-      <c r="T35" s="74"/>
+      <c r="T35" s="85"/>
       <c r="U35" s="46">
         <v>5000</v>
       </c>
@@ -3034,11 +3034,11 @@
       <c r="X35" s="13">
         <v>9</v>
       </c>
-      <c r="Y35" s="93"/>
-      <c r="Z35" s="94"/>
+      <c r="Y35" s="74"/>
+      <c r="Z35" s="75"/>
       <c r="AA35" s="46"/>
-      <c r="AB35" s="86"/>
-      <c r="AC35" s="97"/>
+      <c r="AB35" s="67"/>
+      <c r="AC35" s="68"/>
       <c r="AH35" s="56"/>
     </row>
     <row r="36" spans="7:41" x14ac:dyDescent="0.35">
@@ -3048,20 +3048,20 @@
       <c r="M36" s="15">
         <v>10</v>
       </c>
-      <c r="N36" s="74" t="s">
+      <c r="N36" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="O36" s="74"/>
+      <c r="O36" s="85"/>
       <c r="P36" s="16">
         <v>102000</v>
       </c>
       <c r="R36" s="13">
         <v>10</v>
       </c>
-      <c r="S36" s="77">
+      <c r="S36" s="84">
         <v>45700</v>
       </c>
-      <c r="T36" s="74"/>
+      <c r="T36" s="85"/>
       <c r="U36" s="46">
         <v>5000</v>
       </c>
@@ -3071,11 +3071,11 @@
       <c r="X36" s="13">
         <v>10</v>
       </c>
-      <c r="Y36" s="93"/>
-      <c r="Z36" s="94"/>
+      <c r="Y36" s="74"/>
+      <c r="Z36" s="75"/>
       <c r="AA36" s="46"/>
-      <c r="AB36" s="86"/>
-      <c r="AC36" s="97"/>
+      <c r="AB36" s="67"/>
+      <c r="AC36" s="68"/>
       <c r="AH36" s="56"/>
     </row>
     <row r="37" spans="7:41" x14ac:dyDescent="0.35">
@@ -3083,16 +3083,16 @@
       <c r="H37" s="28"/>
       <c r="I37" s="32"/>
       <c r="M37" s="15"/>
-      <c r="N37" s="74"/>
-      <c r="O37" s="74"/>
+      <c r="N37" s="85"/>
+      <c r="O37" s="85"/>
       <c r="P37" s="16"/>
       <c r="R37" s="13">
         <v>11</v>
       </c>
-      <c r="S37" s="77">
+      <c r="S37" s="84">
         <v>45701</v>
       </c>
-      <c r="T37" s="74"/>
+      <c r="T37" s="85"/>
       <c r="U37" s="46">
         <v>5000</v>
       </c>
@@ -3102,11 +3102,11 @@
       <c r="X37" s="13">
         <v>11</v>
       </c>
-      <c r="Y37" s="93"/>
-      <c r="Z37" s="94"/>
+      <c r="Y37" s="74"/>
+      <c r="Z37" s="75"/>
       <c r="AA37" s="46"/>
-      <c r="AB37" s="86"/>
-      <c r="AC37" s="97"/>
+      <c r="AB37" s="67"/>
+      <c r="AC37" s="68"/>
       <c r="AH37" s="56"/>
     </row>
     <row r="38" spans="7:41" x14ac:dyDescent="0.35">
@@ -3114,16 +3114,16 @@
       <c r="H38" s="28"/>
       <c r="I38" s="32"/>
       <c r="M38" s="15"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
+      <c r="N38" s="85"/>
+      <c r="O38" s="85"/>
       <c r="P38" s="16"/>
       <c r="R38" s="13">
         <v>12</v>
       </c>
-      <c r="S38" s="77">
+      <c r="S38" s="84">
         <v>45702</v>
       </c>
-      <c r="T38" s="74"/>
+      <c r="T38" s="85"/>
       <c r="U38" s="46">
         <v>5000</v>
       </c>
@@ -3133,11 +3133,11 @@
       <c r="X38" s="13">
         <v>12</v>
       </c>
-      <c r="Y38" s="93"/>
-      <c r="Z38" s="94"/>
+      <c r="Y38" s="74"/>
+      <c r="Z38" s="75"/>
       <c r="AA38" s="46"/>
-      <c r="AB38" s="86"/>
-      <c r="AC38" s="97"/>
+      <c r="AB38" s="67"/>
+      <c r="AC38" s="68"/>
       <c r="AH38" s="56"/>
     </row>
     <row r="39" spans="7:41" x14ac:dyDescent="0.35">
@@ -3145,16 +3145,16 @@
       <c r="H39" s="28"/>
       <c r="I39" s="32"/>
       <c r="M39" s="15"/>
-      <c r="N39" s="74"/>
-      <c r="O39" s="74"/>
+      <c r="N39" s="85"/>
+      <c r="O39" s="85"/>
       <c r="P39" s="16"/>
       <c r="R39" s="13">
         <v>13</v>
       </c>
-      <c r="S39" s="77">
+      <c r="S39" s="84">
         <v>45703</v>
       </c>
-      <c r="T39" s="74"/>
+      <c r="T39" s="85"/>
       <c r="U39" s="46">
         <v>5000</v>
       </c>
@@ -3164,11 +3164,11 @@
       <c r="X39" s="13">
         <v>13</v>
       </c>
-      <c r="Y39" s="93"/>
-      <c r="Z39" s="94"/>
+      <c r="Y39" s="74"/>
+      <c r="Z39" s="75"/>
       <c r="AA39" s="46"/>
-      <c r="AB39" s="86"/>
-      <c r="AC39" s="97"/>
+      <c r="AB39" s="67"/>
+      <c r="AC39" s="68"/>
       <c r="AH39" s="56"/>
     </row>
     <row r="40" spans="7:41" x14ac:dyDescent="0.35">
@@ -3176,16 +3176,16 @@
       <c r="H40" s="28"/>
       <c r="I40" s="32"/>
       <c r="M40" s="15"/>
-      <c r="N40" s="74"/>
-      <c r="O40" s="74"/>
+      <c r="N40" s="85"/>
+      <c r="O40" s="85"/>
       <c r="P40" s="16"/>
       <c r="R40" s="13">
         <v>14</v>
       </c>
-      <c r="S40" s="77">
+      <c r="S40" s="84">
         <v>45704</v>
       </c>
-      <c r="T40" s="74"/>
+      <c r="T40" s="85"/>
       <c r="U40" s="46">
         <v>5000</v>
       </c>
@@ -3195,11 +3195,11 @@
       <c r="X40" s="13">
         <v>14</v>
       </c>
-      <c r="Y40" s="93"/>
-      <c r="Z40" s="94"/>
+      <c r="Y40" s="74"/>
+      <c r="Z40" s="75"/>
       <c r="AA40" s="46"/>
-      <c r="AB40" s="86"/>
-      <c r="AC40" s="97"/>
+      <c r="AB40" s="67"/>
+      <c r="AC40" s="68"/>
       <c r="AH40" s="56"/>
     </row>
     <row r="41" spans="7:41" x14ac:dyDescent="0.35">
@@ -3207,16 +3207,16 @@
       <c r="H41" s="28"/>
       <c r="I41" s="32"/>
       <c r="M41" s="15"/>
-      <c r="N41" s="74"/>
-      <c r="O41" s="74"/>
+      <c r="N41" s="85"/>
+      <c r="O41" s="85"/>
       <c r="P41" s="16"/>
       <c r="R41" s="13">
         <v>15</v>
       </c>
-      <c r="S41" s="77">
+      <c r="S41" s="84">
         <v>45705</v>
       </c>
-      <c r="T41" s="74"/>
+      <c r="T41" s="85"/>
       <c r="U41" s="46">
         <v>5000</v>
       </c>
@@ -3226,11 +3226,11 @@
       <c r="X41" s="13">
         <v>15</v>
       </c>
-      <c r="Y41" s="93"/>
-      <c r="Z41" s="94"/>
+      <c r="Y41" s="74"/>
+      <c r="Z41" s="75"/>
       <c r="AA41" s="46"/>
-      <c r="AB41" s="86"/>
-      <c r="AC41" s="97"/>
+      <c r="AB41" s="67"/>
+      <c r="AC41" s="68"/>
       <c r="AH41" s="56"/>
     </row>
     <row r="42" spans="7:41" x14ac:dyDescent="0.35">
@@ -3238,16 +3238,16 @@
       <c r="H42" s="28"/>
       <c r="I42" s="32"/>
       <c r="M42" s="15"/>
-      <c r="N42" s="74"/>
-      <c r="O42" s="74"/>
+      <c r="N42" s="85"/>
+      <c r="O42" s="85"/>
       <c r="P42" s="16"/>
       <c r="R42" s="13">
         <v>16</v>
       </c>
-      <c r="S42" s="77">
+      <c r="S42" s="84">
         <v>45707</v>
       </c>
-      <c r="T42" s="74"/>
+      <c r="T42" s="85"/>
       <c r="U42" s="46">
         <v>5000</v>
       </c>
@@ -3257,11 +3257,11 @@
       <c r="X42" s="13">
         <v>16</v>
       </c>
-      <c r="Y42" s="93"/>
-      <c r="Z42" s="94"/>
+      <c r="Y42" s="74"/>
+      <c r="Z42" s="75"/>
       <c r="AA42" s="46"/>
-      <c r="AB42" s="86"/>
-      <c r="AC42" s="97"/>
+      <c r="AB42" s="67"/>
+      <c r="AC42" s="68"/>
       <c r="AH42" s="56"/>
     </row>
     <row r="43" spans="7:41" x14ac:dyDescent="0.35">
@@ -3269,16 +3269,16 @@
       <c r="H43" s="28"/>
       <c r="I43" s="32"/>
       <c r="M43" s="15"/>
-      <c r="N43" s="74"/>
-      <c r="O43" s="74"/>
+      <c r="N43" s="85"/>
+      <c r="O43" s="85"/>
       <c r="P43" s="16"/>
       <c r="R43" s="13">
         <v>17</v>
       </c>
-      <c r="S43" s="77">
+      <c r="S43" s="84">
         <v>45708</v>
       </c>
-      <c r="T43" s="74"/>
+      <c r="T43" s="85"/>
       <c r="U43" s="46">
         <v>5000</v>
       </c>
@@ -3288,11 +3288,11 @@
       <c r="X43" s="13">
         <v>17</v>
       </c>
-      <c r="Y43" s="93"/>
-      <c r="Z43" s="94"/>
+      <c r="Y43" s="74"/>
+      <c r="Z43" s="75"/>
       <c r="AA43" s="46"/>
-      <c r="AB43" s="86"/>
-      <c r="AC43" s="97"/>
+      <c r="AB43" s="67"/>
+      <c r="AC43" s="68"/>
       <c r="AH43" s="56"/>
     </row>
     <row r="44" spans="7:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3300,16 +3300,16 @@
       <c r="H44" s="29"/>
       <c r="I44" s="34"/>
       <c r="M44" s="15"/>
-      <c r="N44" s="74"/>
-      <c r="O44" s="74"/>
+      <c r="N44" s="85"/>
+      <c r="O44" s="85"/>
       <c r="P44" s="16"/>
       <c r="R44" s="13">
         <v>18</v>
       </c>
-      <c r="S44" s="77">
+      <c r="S44" s="84">
         <v>45709</v>
       </c>
-      <c r="T44" s="74"/>
+      <c r="T44" s="85"/>
       <c r="U44" s="46">
         <v>5000</v>
       </c>
@@ -3319,11 +3319,11 @@
       <c r="X44" s="13">
         <v>18</v>
       </c>
-      <c r="Y44" s="93"/>
-      <c r="Z44" s="94"/>
+      <c r="Y44" s="74"/>
+      <c r="Z44" s="75"/>
       <c r="AA44" s="46"/>
-      <c r="AB44" s="86"/>
-      <c r="AC44" s="97"/>
+      <c r="AB44" s="67"/>
+      <c r="AC44" s="68"/>
       <c r="AH44" s="56"/>
     </row>
     <row r="45" spans="7:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3333,19 +3333,19 @@
       </c>
       <c r="I45" s="35">
         <f>SUM(I28:I44)</f>
-        <v>235500</v>
+        <v>246500</v>
       </c>
       <c r="M45" s="15"/>
-      <c r="N45" s="74"/>
-      <c r="O45" s="74"/>
+      <c r="N45" s="85"/>
+      <c r="O45" s="85"/>
       <c r="P45" s="16"/>
       <c r="R45" s="13">
         <v>19</v>
       </c>
-      <c r="S45" s="77">
+      <c r="S45" s="84">
         <v>45710</v>
       </c>
-      <c r="T45" s="74"/>
+      <c r="T45" s="85"/>
       <c r="U45" s="46">
         <v>5000</v>
       </c>
@@ -3355,25 +3355,25 @@
       <c r="X45" s="13">
         <v>19</v>
       </c>
-      <c r="Y45" s="93"/>
-      <c r="Z45" s="94"/>
+      <c r="Y45" s="74"/>
+      <c r="Z45" s="75"/>
       <c r="AA45" s="46"/>
-      <c r="AB45" s="86"/>
-      <c r="AC45" s="97"/>
+      <c r="AB45" s="67"/>
+      <c r="AC45" s="68"/>
       <c r="AH45" s="56"/>
     </row>
     <row r="46" spans="7:41" x14ac:dyDescent="0.35">
       <c r="M46" s="15"/>
-      <c r="N46" s="74"/>
-      <c r="O46" s="74"/>
+      <c r="N46" s="85"/>
+      <c r="O46" s="85"/>
       <c r="P46" s="16"/>
       <c r="R46" s="13">
         <v>20</v>
       </c>
-      <c r="S46" s="77">
+      <c r="S46" s="84">
         <v>45711</v>
       </c>
-      <c r="T46" s="74"/>
+      <c r="T46" s="85"/>
       <c r="U46" s="46">
         <v>5000</v>
       </c>
@@ -3383,25 +3383,25 @@
       <c r="X46" s="13">
         <v>20</v>
       </c>
-      <c r="Y46" s="93"/>
-      <c r="Z46" s="94"/>
+      <c r="Y46" s="74"/>
+      <c r="Z46" s="75"/>
       <c r="AA46" s="46"/>
-      <c r="AB46" s="86"/>
-      <c r="AC46" s="97"/>
+      <c r="AB46" s="67"/>
+      <c r="AC46" s="68"/>
       <c r="AH46" s="56"/>
     </row>
     <row r="47" spans="7:41" x14ac:dyDescent="0.35">
       <c r="M47" s="15"/>
-      <c r="N47" s="74"/>
-      <c r="O47" s="74"/>
+      <c r="N47" s="85"/>
+      <c r="O47" s="85"/>
       <c r="P47" s="16"/>
       <c r="R47" s="13">
         <v>21</v>
       </c>
-      <c r="S47" s="77">
+      <c r="S47" s="84">
         <v>45712</v>
       </c>
-      <c r="T47" s="74"/>
+      <c r="T47" s="85"/>
       <c r="U47" s="46">
         <v>5000</v>
       </c>
@@ -3411,25 +3411,25 @@
       <c r="X47" s="13">
         <v>21</v>
       </c>
-      <c r="Y47" s="93"/>
-      <c r="Z47" s="94"/>
+      <c r="Y47" s="74"/>
+      <c r="Z47" s="75"/>
       <c r="AA47" s="46"/>
-      <c r="AB47" s="86"/>
-      <c r="AC47" s="97"/>
+      <c r="AB47" s="67"/>
+      <c r="AC47" s="68"/>
       <c r="AH47" s="56"/>
     </row>
     <row r="48" spans="7:41" x14ac:dyDescent="0.35">
       <c r="M48" s="15"/>
-      <c r="N48" s="74"/>
-      <c r="O48" s="74"/>
+      <c r="N48" s="85"/>
+      <c r="O48" s="85"/>
       <c r="P48" s="16"/>
       <c r="R48" s="13">
         <v>22</v>
       </c>
-      <c r="S48" s="77">
+      <c r="S48" s="84">
         <v>45713</v>
       </c>
-      <c r="T48" s="74"/>
+      <c r="T48" s="85"/>
       <c r="U48" s="46">
         <v>5000</v>
       </c>
@@ -3439,25 +3439,25 @@
       <c r="X48" s="13">
         <v>22</v>
       </c>
-      <c r="Y48" s="93"/>
-      <c r="Z48" s="94"/>
+      <c r="Y48" s="74"/>
+      <c r="Z48" s="75"/>
       <c r="AA48" s="46"/>
-      <c r="AB48" s="86"/>
-      <c r="AC48" s="97"/>
+      <c r="AB48" s="67"/>
+      <c r="AC48" s="68"/>
       <c r="AH48" s="56"/>
     </row>
     <row r="49" spans="13:34" x14ac:dyDescent="0.35">
       <c r="M49" s="15"/>
-      <c r="N49" s="74"/>
-      <c r="O49" s="74"/>
+      <c r="N49" s="85"/>
+      <c r="O49" s="85"/>
       <c r="P49" s="16"/>
       <c r="R49" s="13">
         <v>23</v>
       </c>
-      <c r="S49" s="77">
+      <c r="S49" s="84">
         <v>45714</v>
       </c>
-      <c r="T49" s="74"/>
+      <c r="T49" s="85"/>
       <c r="U49" s="46">
         <v>5000</v>
       </c>
@@ -3467,25 +3467,25 @@
       <c r="X49" s="13">
         <v>23</v>
       </c>
-      <c r="Y49" s="93"/>
-      <c r="Z49" s="94"/>
+      <c r="Y49" s="74"/>
+      <c r="Z49" s="75"/>
       <c r="AA49" s="46"/>
-      <c r="AB49" s="86"/>
-      <c r="AC49" s="97"/>
+      <c r="AB49" s="67"/>
+      <c r="AC49" s="68"/>
       <c r="AH49" s="56"/>
     </row>
     <row r="50" spans="13:34" x14ac:dyDescent="0.35">
       <c r="M50" s="15"/>
-      <c r="N50" s="74"/>
-      <c r="O50" s="74"/>
+      <c r="N50" s="85"/>
+      <c r="O50" s="85"/>
       <c r="P50" s="16"/>
       <c r="R50" s="13">
         <v>24</v>
       </c>
-      <c r="S50" s="77">
+      <c r="S50" s="84">
         <v>45716</v>
       </c>
-      <c r="T50" s="74"/>
+      <c r="T50" s="85"/>
       <c r="U50" s="46">
         <v>5000</v>
       </c>
@@ -3495,25 +3495,25 @@
       <c r="X50" s="13">
         <v>24</v>
       </c>
-      <c r="Y50" s="93"/>
-      <c r="Z50" s="94"/>
+      <c r="Y50" s="74"/>
+      <c r="Z50" s="75"/>
       <c r="AA50" s="46"/>
-      <c r="AB50" s="86"/>
-      <c r="AC50" s="97"/>
+      <c r="AB50" s="67"/>
+      <c r="AC50" s="68"/>
       <c r="AH50" s="56"/>
     </row>
     <row r="51" spans="13:34" x14ac:dyDescent="0.35">
       <c r="M51" s="15"/>
-      <c r="N51" s="74"/>
-      <c r="O51" s="74"/>
+      <c r="N51" s="85"/>
+      <c r="O51" s="85"/>
       <c r="P51" s="16"/>
       <c r="R51" s="13">
         <v>25</v>
       </c>
-      <c r="S51" s="77">
+      <c r="S51" s="84">
         <v>45719</v>
       </c>
-      <c r="T51" s="74"/>
+      <c r="T51" s="85"/>
       <c r="U51" s="46">
         <v>5000</v>
       </c>
@@ -3523,25 +3523,25 @@
       <c r="X51" s="13">
         <v>25</v>
       </c>
-      <c r="Y51" s="93"/>
-      <c r="Z51" s="94"/>
+      <c r="Y51" s="74"/>
+      <c r="Z51" s="75"/>
       <c r="AA51" s="46"/>
-      <c r="AB51" s="86"/>
-      <c r="AC51" s="97"/>
+      <c r="AB51" s="67"/>
+      <c r="AC51" s="68"/>
       <c r="AH51" s="56"/>
     </row>
     <row r="52" spans="13:34" x14ac:dyDescent="0.35">
       <c r="M52" s="15"/>
-      <c r="N52" s="74"/>
-      <c r="O52" s="74"/>
+      <c r="N52" s="85"/>
+      <c r="O52" s="85"/>
       <c r="P52" s="16"/>
       <c r="R52" s="13">
         <v>26</v>
       </c>
-      <c r="S52" s="77">
+      <c r="S52" s="84">
         <v>45723</v>
       </c>
-      <c r="T52" s="74"/>
+      <c r="T52" s="85"/>
       <c r="U52" s="46">
         <v>5000</v>
       </c>
@@ -3551,25 +3551,25 @@
       <c r="X52" s="13">
         <v>26</v>
       </c>
-      <c r="Y52" s="93"/>
-      <c r="Z52" s="94"/>
+      <c r="Y52" s="74"/>
+      <c r="Z52" s="75"/>
       <c r="AA52" s="46"/>
-      <c r="AB52" s="86"/>
-      <c r="AC52" s="97"/>
+      <c r="AB52" s="67"/>
+      <c r="AC52" s="68"/>
       <c r="AH52" s="56"/>
     </row>
     <row r="53" spans="13:34" x14ac:dyDescent="0.35">
       <c r="M53" s="15"/>
-      <c r="N53" s="86"/>
-      <c r="O53" s="87"/>
+      <c r="N53" s="67"/>
+      <c r="O53" s="86"/>
       <c r="P53" s="16"/>
       <c r="R53" s="13">
         <v>27</v>
       </c>
-      <c r="S53" s="77">
+      <c r="S53" s="84">
         <v>45724</v>
       </c>
-      <c r="T53" s="74"/>
+      <c r="T53" s="85"/>
       <c r="U53" s="46">
         <v>5000</v>
       </c>
@@ -3579,25 +3579,25 @@
       <c r="X53" s="13">
         <v>27</v>
       </c>
-      <c r="Y53" s="93"/>
-      <c r="Z53" s="94"/>
+      <c r="Y53" s="74"/>
+      <c r="Z53" s="75"/>
       <c r="AA53" s="46"/>
-      <c r="AB53" s="86"/>
-      <c r="AC53" s="97"/>
+      <c r="AB53" s="67"/>
+      <c r="AC53" s="68"/>
       <c r="AH53" s="56"/>
     </row>
     <row r="54" spans="13:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="M54" s="39"/>
-      <c r="N54" s="88"/>
-      <c r="O54" s="89"/>
+      <c r="N54" s="87"/>
+      <c r="O54" s="88"/>
       <c r="P54" s="40"/>
       <c r="R54" s="13">
         <v>28</v>
       </c>
-      <c r="S54" s="77">
+      <c r="S54" s="84">
         <v>45726</v>
       </c>
-      <c r="T54" s="74"/>
+      <c r="T54" s="85"/>
       <c r="U54" s="46">
         <v>10000</v>
       </c>
@@ -3607,42 +3607,42 @@
       <c r="X54" s="13">
         <v>28</v>
       </c>
-      <c r="Y54" s="104"/>
-      <c r="Z54" s="105"/>
+      <c r="Y54" s="76"/>
+      <c r="Z54" s="77"/>
       <c r="AA54" s="46"/>
-      <c r="AB54" s="86"/>
-      <c r="AC54" s="97"/>
+      <c r="AB54" s="67"/>
+      <c r="AC54" s="68"/>
     </row>
     <row r="55" spans="13:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="M55" s="67" t="s">
+      <c r="M55" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="N55" s="68"/>
-      <c r="O55" s="90"/>
+      <c r="N55" s="70"/>
+      <c r="O55" s="71"/>
       <c r="P55" s="41">
         <f>SUM(P27:P54)</f>
         <v>720500</v>
       </c>
-      <c r="R55" s="67" t="s">
+      <c r="R55" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="S55" s="68"/>
-      <c r="T55" s="90"/>
+      <c r="S55" s="70"/>
+      <c r="T55" s="71"/>
       <c r="U55" s="47">
         <f>SUM(U27:U54)</f>
         <v>145000</v>
       </c>
       <c r="V55" s="44"/>
-      <c r="X55" s="67" t="s">
+      <c r="X55" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="Y55" s="68"/>
-      <c r="Z55" s="90"/>
-      <c r="AA55" s="102">
+      <c r="Y55" s="70"/>
+      <c r="Z55" s="71"/>
+      <c r="AA55" s="72">
         <f>SUM(AA27:AA54)</f>
         <v>40000</v>
       </c>
-      <c r="AB55" s="103"/>
+      <c r="AB55" s="73"/>
       <c r="AC55" s="57"/>
     </row>
   </sheetData>
@@ -3650,31 +3650,106 @@
     <sortCondition ref="AH26:AH53"/>
   </sortState>
   <mergeCells count="149">
-    <mergeCell ref="AB39:AC39"/>
-    <mergeCell ref="AB40:AC40"/>
-    <mergeCell ref="AB41:AC41"/>
-    <mergeCell ref="AB52:AC52"/>
-    <mergeCell ref="AB53:AC53"/>
-    <mergeCell ref="AB54:AC54"/>
-    <mergeCell ref="X55:Z55"/>
-    <mergeCell ref="AA55:AB55"/>
-    <mergeCell ref="AB47:AC47"/>
-    <mergeCell ref="AB48:AC48"/>
-    <mergeCell ref="AB49:AC49"/>
-    <mergeCell ref="AB50:AC50"/>
-    <mergeCell ref="AB51:AC51"/>
-    <mergeCell ref="Y52:Z52"/>
-    <mergeCell ref="Y53:Z53"/>
-    <mergeCell ref="Y54:Z54"/>
-    <mergeCell ref="AB26:AC26"/>
-    <mergeCell ref="AB27:AC27"/>
-    <mergeCell ref="AB28:AC28"/>
-    <mergeCell ref="AB29:AC29"/>
-    <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="AB31:AC31"/>
-    <mergeCell ref="AB32:AC32"/>
-    <mergeCell ref="AB33:AC33"/>
-    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="AQ3:AT3"/>
+    <mergeCell ref="AQ22:AR22"/>
+    <mergeCell ref="AS22:AT22"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="AG3:AJ3"/>
+    <mergeCell ref="AG22:AH22"/>
+    <mergeCell ref="AI22:AJ22"/>
+    <mergeCell ref="AL3:AO3"/>
+    <mergeCell ref="AL22:AM22"/>
+    <mergeCell ref="AN22:AO22"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="AB3:AE3"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="AD22:AE22"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R25:U25"/>
+    <mergeCell ref="N53:O53"/>
+    <mergeCell ref="N54:O54"/>
+    <mergeCell ref="M55:O55"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="N51:O51"/>
+    <mergeCell ref="N52:O52"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="R55:T55"/>
+    <mergeCell ref="S46:T46"/>
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="S49:T49"/>
+    <mergeCell ref="S50:T50"/>
+    <mergeCell ref="S32:T32"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="S51:T51"/>
+    <mergeCell ref="S52:T52"/>
+    <mergeCell ref="S53:T53"/>
+    <mergeCell ref="S54:T54"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="S45:T45"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="S37:T37"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S39:T39"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="Y32:Z32"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="Y35:Z35"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="Y29:Z29"/>
+    <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="Y31:Z31"/>
     <mergeCell ref="AB35:AC35"/>
     <mergeCell ref="AB36:AC36"/>
     <mergeCell ref="Y47:Z47"/>
@@ -3699,106 +3774,31 @@
     <mergeCell ref="AB46:AC46"/>
     <mergeCell ref="AB37:AC37"/>
     <mergeCell ref="AB38:AC38"/>
-    <mergeCell ref="Y32:Z32"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="Y35:Z35"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="Y27:Z27"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="Y31:Z31"/>
-    <mergeCell ref="R55:T55"/>
-    <mergeCell ref="S46:T46"/>
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="S49:T49"/>
-    <mergeCell ref="S50:T50"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="S35:T35"/>
-    <mergeCell ref="S51:T51"/>
-    <mergeCell ref="S52:T52"/>
-    <mergeCell ref="S53:T53"/>
-    <mergeCell ref="S54:T54"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="S45:T45"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="S37:T37"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S39:T39"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="N53:O53"/>
-    <mergeCell ref="N54:O54"/>
-    <mergeCell ref="M55:O55"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="N50:O50"/>
-    <mergeCell ref="N51:O51"/>
-    <mergeCell ref="N52:O52"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="AQ3:AT3"/>
-    <mergeCell ref="AQ22:AR22"/>
-    <mergeCell ref="AS22:AT22"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="AG3:AJ3"/>
-    <mergeCell ref="AG22:AH22"/>
-    <mergeCell ref="AI22:AJ22"/>
-    <mergeCell ref="AL3:AO3"/>
-    <mergeCell ref="AL22:AM22"/>
-    <mergeCell ref="AN22:AO22"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="AB3:AE3"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="AD22:AE22"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R25:U25"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="AB27:AC27"/>
+    <mergeCell ref="AB28:AC28"/>
+    <mergeCell ref="AB29:AC29"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AB32:AC32"/>
+    <mergeCell ref="AB33:AC33"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="AB39:AC39"/>
+    <mergeCell ref="AB40:AC40"/>
+    <mergeCell ref="AB41:AC41"/>
+    <mergeCell ref="AB52:AC52"/>
+    <mergeCell ref="AB53:AC53"/>
+    <mergeCell ref="AB54:AC54"/>
+    <mergeCell ref="X55:Z55"/>
+    <mergeCell ref="AA55:AB55"/>
+    <mergeCell ref="AB47:AC47"/>
+    <mergeCell ref="AB48:AC48"/>
+    <mergeCell ref="AB49:AC49"/>
+    <mergeCell ref="AB50:AC50"/>
+    <mergeCell ref="AB51:AC51"/>
+    <mergeCell ref="Y52:Z52"/>
+    <mergeCell ref="Y53:Z53"/>
+    <mergeCell ref="Y54:Z54"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>